<commit_message>
Tournament stage + Chart Update
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karol\Desktop\Gdynia_IV_SEM\AI\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karol\Desktop\GE_tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D621A5D-8B16-45ED-B85A-509EDB0767DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6C7B13-299D-4F24-8A47-70FF47B8857D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26B64432-B301-4B69-BDDD-D721FDDAF1F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>15 min</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Krzyżowanie</t>
   </si>
   <si>
-    <t>? - selekcja 3</t>
-  </si>
-  <si>
     <t>zapis danych do plików</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Steady State - selekcja 2</t>
+  </si>
+  <si>
+    <t>Tournament - selekcja 3</t>
   </si>
 </sst>
 </file>
@@ -189,19 +189,19 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -516,19 +516,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5765B20F-DDB6-4FB7-BC36-ADF2292B96B5}">
-  <dimension ref="C4:Z29"/>
+  <dimension ref="C4:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3" t="s">
+    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -591,16 +591,25 @@
       <c r="Z4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="AA4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -619,17 +628,20 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+    </row>
+    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -647,18 +659,21 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -675,19 +690,22 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -703,21 +721,24 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -731,13 +752,16 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -746,7 +770,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="5"/>
+      <c r="N10" s="3"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -759,13 +783,16 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-    </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -775,10 +802,10 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -787,13 +814,16 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-    </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -810,18 +840,21 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
-      <c r="V12" s="9"/>
+      <c r="V12" s="7"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-    </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -839,17 +872,20 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
       <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -871,13 +907,16 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -899,54 +938,67 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="5"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="6"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="7"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
@@ -955,16 +1007,6 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>